<commit_message>
new site forms on vc and habr
</commit_message>
<xml_diff>
--- a/data/news.xlsx
+++ b/data/news.xlsx
@@ -511,33 +511,57 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>725</v>
-      </c>
-      <c r="C2" t="inlineStr"/>
+        <v>1973</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ПБ</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Использование CROSS JOIN для задач поиска пересечений в исторических данных</t>
+          <t>Использование библиотеки Facerecognition и фреймворка Django для распознавания лиц в реальном времени</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>07.08.2023</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+          <t>11.08.2023</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>ББ</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ВВБ</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Белова Елена Витальевна</t>
+        </is>
+      </c>
       <c r="I2" t="n">
-        <v>0.26</v>
+        <v>1</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Обработка записей разговоров на Python. Поиск пересечений в диалоге</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
+          <t>Использование библиотеки Facerecognition и фреймворка Django для распознавания лиц в реальном времени</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>1973</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Использование библиотеки facerecognition и фреймворка Django для распознавания лиц в реальном времени.</t>
+        </is>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>45110</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -546,56 +570,56 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1947</v>
+        <v>1976</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ЦЧБ</t>
+          <t>СибБ</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Как найти младенца или выжить на Титанике? Возможности формул и функций в Power Query Excel для анализа данных.</t>
+          <t>Microsoft Bing и ChatGPT - buddy DA-DS-аудитора</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>09.08.2023</t>
+          <t>15.08.2023</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>СЗБ</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>ББ</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>МБ</t>
-        </is>
-      </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Оганесян Евгения Викторовна</t>
+          <t>Шайдурова Арина Владимировна</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Как найти младенца или выжить на Титанике?</t>
+          <t>Microsoft Bing и ChatGPT - buddy DA-DS-аудитора</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>1947</v>
+        <v>1976</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Как найти младенца или выжить на Титанике? Возможности формул и функций в Power Query Excel для анализа данных (1908)</t>
+          <t>Microsoft Bing и ChatGPT - buddy будущего</t>
         </is>
       </c>
       <c r="M3" s="2" t="n">
-        <v>44995</v>
+        <v>45030</v>
       </c>
     </row>
     <row r="4">
@@ -605,36 +629,36 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1973</v>
+        <v>1974</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ПБ</t>
+          <t>СРБ</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Использование библиотеки Facerecognition и фреймворка Django для распознавания лиц в реальном времени</t>
+          <t>Как скачать отчёты из Power BI на диск с помощью PowerShell</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>11.08.2023</t>
+          <t>17.08.2023</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ББ</t>
+          <t>СЗБ</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>ВВБ</t>
+          <t>ЦЧБ</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Белова Елена Витальевна</t>
+          <t>Ермолаева Светлана Алексеевна</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -642,78 +666,78 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Использование библиотеки Facerecognition и фреймворка Django для распознавания лиц в реальном времени</t>
+          <t>Как скачать отчёты из Power BI на диск с помощью PowerShell</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>1973</v>
+        <v>1974</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Использование библиотеки facerecognition и фреймворка Django для распознавания лиц в реальном времени.</t>
+          <t>Как сохранить все отчёты с сервера Power BI</t>
         </is>
       </c>
       <c r="M4" s="2" t="n">
-        <v>45110</v>
+        <v>45079</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SDrug</t>
+          <t>Habr</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1977</v>
+        <v>1965</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ПБ</t>
+          <t>ЦЧБ</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Кодируй, властвуй, визуализируй!</t>
+          <t>Замена Paint в задачах разметки графических данных</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>08.08.2023</t>
+          <t>14.08.2023</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>УБ</t>
+          <t>ЮЗБ</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>СибБ</t>
+          <t>МБ</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Вальдман Анна Аркадьевна</t>
+          <t>Ермолаева Светлана Алексеевна</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0.79</v>
+        <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Кодируй и визуализируй</t>
+          <t>Замена Paint в задачах разметки графических данных</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>1977</v>
+        <v>1965</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Кодируй, властвуй, визуализируй!</t>
+          <t>Замена paint в задачах разметки графических данных</t>
         </is>
       </c>
       <c r="M5" s="2" t="n">
-        <v>45026</v>
+        <v>45062</v>
       </c>
     </row>
   </sheetData>

</xml_diff>